<commit_message>
Commiting changes after incorporating events for video pages
</commit_message>
<xml_diff>
--- a/Files/Events/Events.xlsx
+++ b/Files/Events/Events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahota\Documents\Work\Selenium\GA\Events\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahota\PycharmProjects\GA\Files\Events\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1E2703-DEBE-4472-8F2A-AC813328CDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB0C564-0726-47BB-868B-687E233CA5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="TAXONOMY" sheetId="3" r:id="rId4"/>
     <sheet name="BIO" sheetId="10" r:id="rId5"/>
     <sheet name="LISTSC" sheetId="9" r:id="rId6"/>
+    <sheet name="GENERALVIDEO" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>className</t>
   </si>
@@ -45,13 +46,31 @@
   </si>
   <si>
     <t>share-link share-link-facebook</t>
+  </si>
+  <si>
+    <t>comp js-rating-button button--outlined-little-round article-feedback__rating-button article-feedback__thumbs-up-button mntl-button</t>
+  </si>
+  <si>
+    <t>comp mntl-card-list-items mntl-document-card mntl-card card card--no-image</t>
+  </si>
+  <si>
+    <t>jumpstart-control jumpstart-control-pause</t>
+  </si>
+  <si>
+    <t>jumpstart-control jumpstart-control-play</t>
+  </si>
+  <si>
+    <t>jumpstart-control jumpstart-control-mute</t>
+  </si>
+  <si>
+    <t>jumpstart-control jumpstart-control-unmute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,16 +81,48 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF067D17"/>
-      <name val="JetBrains Mono"/>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,10 +145,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -383,40 +452,36 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -430,38 +495,40 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>100</v>
       </c>
     </row>
@@ -476,38 +543,40 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>100</v>
       </c>
     </row>
@@ -526,35 +595,37 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>100</v>
       </c>
     </row>
@@ -568,41 +639,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC0AD16-FBE6-4EB0-ADA1-4A54E9ACCA26}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
+      <c r="B3" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -612,43 +681,125 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85377AE0-68B7-46C2-B5D5-EBE24CA65E7B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A3" sqref="A3:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="121.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>9900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837B892A-158B-471D-9D6A-5B905D6E5D8D}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: uncomment some lines and revert project state to working state
</commit_message>
<xml_diff>
--- a/Files/Events/Events.xlsx
+++ b/Files/Events/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahota\PycharmProjects\GA\Files\Events\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB0C564-0726-47BB-868B-687E233CA5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA7354D-5B7B-4FB1-9E30-07E2E222F7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GENERAL" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="13">
   <si>
     <t>className</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>jumpstart-control jumpstart-control-unmute</t>
+  </si>
+  <si>
+    <t>comp card--featured mntl-document-card mntl-card card card--no-image</t>
+  </si>
+  <si>
+    <t>newsletter-dialog-footer-link dialog-link mntl-text-link footer__newsletter-link</t>
   </si>
 </sst>
 </file>
@@ -145,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -168,6 +174,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,23 +604,23 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9A6F56-9060-4F50-ADB7-6B958DA3E766}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -613,20 +628,30 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1"/>
+      <c r="A4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="11">
+        <v>13000</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>100</v>
+      <c r="A5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="11">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -752,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837B892A-158B-471D-9D6A-5B905D6E5D8D}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>